<commit_message>
Logical functions IF, IFS, AND, OR in excel
</commit_message>
<xml_diff>
--- a/Practice Exel Basics.xlsx
+++ b/Practice Exel Basics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\self projects\New folder\Documents\Exel Practice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57226D46-DA11-46B6-9326-A84DD3955D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7CC4214-7D29-4B55-BFA0-A105EACA18B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="6" activeTab="7" xr2:uid="{38B942BA-1CE7-4988-968E-F31174A453F3}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" firstSheet="8" activeTab="8" xr2:uid="{38B942BA-1CE7-4988-968E-F31174A453F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Basics Excel" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Splitting data" sheetId="6" r:id="rId6"/>
     <sheet name="Data_Validation" sheetId="7" r:id="rId7"/>
     <sheet name="Incentive Calculation" sheetId="8" r:id="rId8"/>
+    <sheet name="Logical Functions" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6558" uniqueCount="2625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6613" uniqueCount="2638">
   <si>
     <t>Employee ID</t>
   </si>
@@ -8017,6 +8018,45 @@
   <si>
     <t>Targert Status</t>
   </si>
+  <si>
+    <t>IFS(D2&gt;75000, D2*20%, D2&gt;50000, D2*15%,D2&lt;50000,D2*10%))</t>
+  </si>
+  <si>
+    <t>IFS is used for multiple conditions</t>
+  </si>
+  <si>
+    <t>Working (years)</t>
+  </si>
+  <si>
+    <t>(And)Promotion</t>
+  </si>
+  <si>
+    <t>(Or) Pro</t>
+  </si>
+  <si>
+    <t>Use of And / Or</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>Promotion</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>5&gt;=</t>
+  </si>
+  <si>
+    <t>Any One</t>
+  </si>
+  <si>
+    <t>finance</t>
+  </si>
+  <si>
+    <t>&gt;5</t>
+  </si>
 </sst>
 </file>
 
@@ -8025,7 +8065,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$₹-861]\ #,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8089,8 +8129,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -8141,6 +8188,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -8255,7 +8308,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -8340,17 +8393,19 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -76573,13 +76628,13 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="30" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="31">
@@ -76587,13 +76642,13 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="30" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="31">
@@ -76601,13 +76656,13 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="30" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="31">
@@ -76615,13 +76670,13 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="30" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="31">
@@ -76629,13 +76684,13 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="30" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="31">
@@ -76643,13 +76698,13 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="30" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="31">
@@ -76657,13 +76712,13 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="30" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="31">
@@ -76671,13 +76726,13 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="30" t="s">
         <v>2606</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="30" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="31">
@@ -76685,30 +76740,30 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="30" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="31">
         <v>9812345686</v>
       </c>
-      <c r="F10" s="36" t="s">
+      <c r="F10" s="30" t="s">
         <v>2609</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="30" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="31">
@@ -76716,13 +76771,13 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="30" t="s">
         <v>2607</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="30" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="31">
@@ -76730,16 +76785,16 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="30" t="s">
         <v>2608</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="35">
+      <c r="D13" s="31">
         <v>9812323245</v>
       </c>
     </row>
@@ -76757,10 +76812,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3F385D8-BCDD-403E-96D2-A6E327893D4D}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -76796,19 +76851,19 @@
         <v>2612</v>
       </c>
       <c r="G1" s="33"/>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="34" t="s">
         <v>2613</v>
       </c>
-      <c r="I1" s="34"/>
+      <c r="I1" s="30"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="30" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="31">
@@ -76823,21 +76878,21 @@
         <v>10905.6</v>
       </c>
       <c r="G2" s="31"/>
-      <c r="H2" s="34" t="s">
+      <c r="H2" s="30" t="s">
         <v>2615</v>
       </c>
-      <c r="I2" s="34" t="s">
+      <c r="I2" s="30" t="s">
         <v>2616</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="30" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="31">
@@ -76852,7 +76907,7 @@
         <v>4471.8</v>
       </c>
       <c r="G3" s="31"/>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="30" t="s">
         <v>2618</v>
       </c>
       <c r="I3" s="32" t="s">
@@ -76860,13 +76915,13 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="34" t="s">
+      <c r="C4" s="30" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="31">
@@ -76881,21 +76936,21 @@
         <v>3521</v>
       </c>
       <c r="G4" s="31"/>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="30" t="s">
         <v>2619</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="30" t="s">
         <v>2617</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="30" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="31">
@@ -76910,17 +76965,17 @@
         <v>3068.1000000000004</v>
       </c>
       <c r="G5" s="31"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="30" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="31">
@@ -76935,17 +76990,17 @@
         <v>4748.7</v>
       </c>
       <c r="G6" s="31"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="30" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="31">
@@ -76960,19 +77015,19 @@
         <v>3000</v>
       </c>
       <c r="G7" s="31"/>
-      <c r="H7" s="38" t="s">
+      <c r="H7" s="36" t="s">
         <v>2620</v>
       </c>
-      <c r="I7" s="38"/>
+      <c r="I7" s="36"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="30" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="31">
@@ -76987,21 +77042,21 @@
         <v>9550.65</v>
       </c>
       <c r="G8" s="31"/>
-      <c r="H8" s="34" t="s">
+      <c r="H8" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="34" t="s">
+      <c r="I8" s="30" t="s">
         <v>2621</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="30" t="s">
         <v>2606</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="30" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="31">
@@ -77016,21 +77071,21 @@
         <v>3896.6000000000004</v>
       </c>
       <c r="G9" s="31"/>
-      <c r="H9" s="34" t="s">
+      <c r="H9" s="30" t="s">
         <v>2622</v>
       </c>
-      <c r="I9" s="39">
+      <c r="I9" s="35">
         <v>0.2</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="34" t="s">
+      <c r="B10" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="30" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="31">
@@ -77045,21 +77100,21 @@
         <v>15410.400000000001</v>
       </c>
       <c r="G10" s="31"/>
-      <c r="H10" s="34" t="s">
+      <c r="H10" s="30" t="s">
         <v>2623</v>
       </c>
-      <c r="I10" s="39">
+      <c r="I10" s="35">
         <v>0.15</v>
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="34" t="s">
+      <c r="C11" s="30" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="31">
@@ -77074,21 +77129,21 @@
         <v>17314</v>
       </c>
       <c r="G11" s="31"/>
-      <c r="H11" s="34" t="s">
+      <c r="H11" s="30" t="s">
         <v>2619</v>
       </c>
-      <c r="I11" s="39">
+      <c r="I11" s="35">
         <v>0.1</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="30" t="s">
         <v>2607</v>
       </c>
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="30" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="31">
@@ -77103,17 +77158,17 @@
         <v>3025</v>
       </c>
       <c r="G12" s="31"/>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="30" t="s">
         <v>2608</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="30" t="s">
         <v>12</v>
       </c>
       <c r="D13" s="31">
@@ -77128,8 +77183,23 @@
         <v>10737.6</v>
       </c>
       <c r="G13" s="31"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="C16" s="38" t="s">
+        <v>2626</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8">
+      <c r="C17" s="37" t="s">
+        <v>2625</v>
+      </c>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37"/>
+      <c r="G17" s="37"/>
+      <c r="H17" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -77137,4 +77207,351 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79DB7AD6-CDE1-46C3-A011-A5031F6E1C0F}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>2627</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>2628</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>2629</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="31">
+        <v>5</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="40" t="str">
+        <f>IF(AND(B2 = "Finance",  C2 &gt;=5),  "Yes", "No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="F2" s="40" t="str">
+        <f>IF(OR(B2 = "Finance", C2&gt;5),"Yes", "No")</f>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="31">
+        <v>4</v>
+      </c>
+      <c r="D3" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="40" t="str">
+        <f t="shared" ref="E3:E13" si="0">IF(AND(B3 = "Finance",  C3 &gt;=5),  "Yes", "No")</f>
+        <v>No</v>
+      </c>
+      <c r="F3" s="40" t="str">
+        <f t="shared" ref="F3:F13" si="1">IF(OR(B3 = "Finance", C3&gt;5),"Yes", "No")</f>
+        <v>No</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>2630</v>
+      </c>
+      <c r="I3" s="38"/>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="31">
+        <v>3</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="F4" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="31">
+        <v>5</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="F5" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="H5" s="41" t="s">
+        <v>2631</v>
+      </c>
+      <c r="I5" s="41"/>
+      <c r="J5" s="40" t="s">
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="31">
+        <v>6</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="F6" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="H6" s="40" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="40" t="s">
+        <v>2634</v>
+      </c>
+      <c r="J6" s="40" t="s">
+        <v>2633</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="31">
+        <v>2</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="F7" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="31">
+        <v>3</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="F8" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>2635</v>
+      </c>
+      <c r="I8" s="41"/>
+      <c r="J8" s="40" t="s">
+        <v>2632</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="31">
+        <v>5</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="F9" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+      <c r="H9" s="40" t="s">
+        <v>2636</v>
+      </c>
+      <c r="I9" s="40" t="s">
+        <v>2637</v>
+      </c>
+      <c r="J9" s="40" t="s">
+        <v>2633</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="31">
+        <v>6</v>
+      </c>
+      <c r="D10" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="F10" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="31">
+        <v>2</v>
+      </c>
+      <c r="D11" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="F11" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>No</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="31">
+        <v>7</v>
+      </c>
+      <c r="D12" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="F12" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="31">
+        <v>7</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="40" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="F13" s="40" t="str">
+        <f t="shared" si="1"/>
+        <v>Yes</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H8:I8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>